<commit_message>
Day 26: Adding header, total price, company name and logo
</commit_message>
<xml_diff>
--- a/invoices/10001-2023.1.18.xlsx
+++ b/invoices/10001-2023.1.18.xlsx
@@ -187,14 +187,15 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="16.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>